<commit_message>
Update DM integration fixture hierarchies
</commit_message>
<xml_diff>
--- a/yti-taxgen-test-commons/src/main/resources/test_fixtures/rds_source_config/dm_integration_fixture/explicit-dimensions-2018-1.xlsx
+++ b/yti-taxgen-test-commons/src/main/resources/test_fixtures/rds_source_config/dm_integration_fixture/explicit-dimensions-2018-1.xlsx
@@ -195,7 +195,7 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>45754185-b964-4112-8fc4-f6d69a1fe881</t>
+          <t>ea439bf8-4eec-4df5-916a-90b144e1d58b</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
@@ -264,7 +264,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="1" customWidth="1" width="34.1"/>
+    <col min="1" max="1" bestFit="1" customWidth="1" width="35.2"/>
     <col min="2" max="2" bestFit="1" customWidth="1" width="18.15"/>
     <col min="3" max="3" bestFit="1" customWidth="1" width="16.5"/>
     <col min="4" max="4" bestFit="1" customWidth="1" width="14.85"/>
@@ -331,7 +331,7 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>9ccf955b-cc12-419c-b039-0ef4e279fef3</t>
+          <t>b042fb98-44f3-41b4-b033-8ad4e766bcf4</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
@@ -367,7 +367,7 @@
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>08172017-95dc-4e6c-b07e-fae9c695c8a8</t>
+          <t>2bcedb0f-6fe3-41d8-a887-c53337b9ce71</t>
         </is>
       </c>
       <c r="B3" s="0" t="inlineStr">
@@ -403,7 +403,7 @@
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>8627d6d9-4270-48ac-ab09-6796331e763c</t>
+          <t>63cd4d2e-cdde-4abb-ae29-6f575b4addbc</t>
         </is>
       </c>
       <c r="B4" s="0" t="inlineStr">
@@ -439,7 +439,7 @@
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>e9f3e1a7-38eb-42c8-bea8-dc7b359730a7</t>
+          <t>c6334b1d-c45e-42e8-9bd9-984576e388bc</t>
         </is>
       </c>
       <c r="B5" s="0" t="inlineStr">
@@ -492,7 +492,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="1" customWidth="1" width="31.900000000000002"/>
+    <col min="1" max="1" bestFit="1" customWidth="1" width="29.700000000000003"/>
     <col min="2" max="2" bestFit="1" customWidth="1" width="18.15"/>
     <col min="3" max="3" bestFit="1" customWidth="1" width="14.85"/>
     <col min="4" max="4" bestFit="1" customWidth="1" width="24.75"/>
@@ -553,7 +553,7 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>4bd7767a-8afd-4317-b401-dc4dba7c4eb8</t>
+          <t>61cd9133-85bf-49df-a4cc-b02f4b7e0cd4</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
@@ -601,7 +601,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="1" customWidth="1" width="34.1"/>
+    <col min="1" max="1" bestFit="1" customWidth="1" width="35.2"/>
     <col min="2" max="2" bestFit="1" customWidth="1" width="11.549999999999999"/>
     <col min="3" max="3" bestFit="1" customWidth="1" width="31.349999999999998"/>
   </cols>
@@ -626,7 +626,7 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>c2d9797f-ae43-4531-ac94-321a70a2739c</t>
+          <t>e363b4d7-504f-4a4b-bed6-41bdb1f03659</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
@@ -643,7 +643,7 @@
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>1ca3c132-e5f3-428b-85db-2379580931b2</t>
+          <t>b03d2cd4-4416-429a-bdaa-e661f7241d30</t>
         </is>
       </c>
       <c r="B3" s="0" t="inlineStr">
@@ -660,7 +660,7 @@
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>03efa971-0985-465b-ae41-1322c7bf6e87</t>
+          <t>7e27e7ca-9ca2-401a-9955-40eea1d8c443</t>
         </is>
       </c>
       <c r="B4" s="0" t="inlineStr">
@@ -677,7 +677,7 @@
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>0571eb0a-fb93-4d12-a97a-1e3fabac269a</t>
+          <t>735c9b13-795a-4328-bba3-7d2b15832476</t>
         </is>
       </c>
       <c r="B5" s="0" t="inlineStr">

</xml_diff>